<commit_message>
Bug fix 4994 and commingle cargo part fix
</commit_message>
<xml_diff>
--- a/api/cp-dss-api/gateway/src/main/resources/reports/loading/Vessel_1_Loading_Plan_Template.xlsx
+++ b/api/cp-dss-api/gateway/src/main/resources/reports/loading/Vessel_1_Loading_Plan_Template.xlsx
@@ -419,21 +419,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F8")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
@@ -444,7 +429,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[0].commingled==false", lastCell="B8", areas=["B7:B8","B94:B95"])</t>
+          <t>Author:
+jx:area(lastCell="B8")
+jx:if(condition="sheetThree.cargoTanks[0].commingled==false", lastCell="B8", areas=["B7:B8","B94:B95"])</t>
         </r>
       </text>
     </comment>
@@ -478,21 +465,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F10")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B9" authorId="0" shapeId="0">
       <text>
         <r>
@@ -503,7 +475,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[1].commingled==false", lastCell="B10", areas=["B9:B10","B96:B97"])</t>
+          <t>Author:
+jx:area(lastCell="B10")
+jx:if(condition="sheetThree.cargoTanks[1].commingled==false", lastCell="B10", areas=["B9:B10","B96:B97"])</t>
         </r>
       </text>
     </comment>
@@ -537,21 +511,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F12")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B11" authorId="0" shapeId="0">
       <text>
         <r>
@@ -562,7 +521,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[2].commingled==false", lastCell="B12", areas=["B11:B12","B98:B99"])</t>
+          <t xml:space="preserve">Author:
+jx:if(condition="sheetThree.cargoTanks[2].commingled ==false", lastCell="B12", areas=["B11:B12","B98:B99"]) </t>
         </r>
       </text>
     </comment>
@@ -596,21 +556,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F14")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B13" authorId="0" shapeId="0">
       <text>
         <r>
@@ -621,7 +566,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[3].commingled == false", lastCell="B14", areas=["B13:B14","B100:B101"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[3].commingled==false", lastCell="B14", areas=["B13:B14","B100:B101"])</t>
         </r>
       </text>
     </comment>
@@ -655,21 +600,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F16")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B15" authorId="0" shapeId="0">
       <text>
         <r>
@@ -680,7 +610,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[4].commingled == false", lastCell="B16", areas=["B15:B16","B102:B103"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[4].commingled==false", lastCell="B16", areas=["B15:B16","B102:B103"])</t>
         </r>
       </text>
     </comment>
@@ -714,21 +644,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A17" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F18")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B17" authorId="0" shapeId="0">
       <text>
         <r>
@@ -739,7 +654,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[5].commingled== false", lastCell="B18", areas=["B17:B18","B104:B105"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[5].commingled==false", lastCell="B18", areas=["B17:B18","B104:B105"])</t>
         </r>
       </text>
     </comment>
@@ -773,21 +688,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F20")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B19" authorId="0" shapeId="0">
       <text>
         <r>
@@ -798,7 +698,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[6].commingled== false", lastCell="B20", areas=["B19:B20","B106:B107"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[6].commingled==false", lastCell="B20", areas=["B19:B20","B106:B107"])</t>
         </r>
       </text>
     </comment>
@@ -832,21 +732,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F22")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B21" authorId="0" shapeId="0">
       <text>
         <r>
@@ -857,7 +742,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[7].commingled== false", lastCell="B22", areas=["B21:B22","B108:B109"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[7].commingled==false", lastCell="B22", areas=["B21:B22","B108:B109"])</t>
         </r>
       </text>
     </comment>
@@ -891,21 +776,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F24")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B23" authorId="0" shapeId="0">
       <text>
         <r>
@@ -916,7 +786,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[8].commingled== false", lastCell="B24", areas=["B23:B24","B110:B111"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[8].commingled==false", lastCell="B24", areas=["B23:B24","B110:B111"])</t>
         </r>
       </text>
     </comment>
@@ -950,21 +820,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F26")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B25" authorId="0" shapeId="0">
       <text>
         <r>
@@ -975,7 +830,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[9].commingled == false", lastCell="B26", areas=["B25:B26","B112:B113"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[9].commingled==false", lastCell="B26", areas=["B25:B26","B112:B113"])</t>
         </r>
       </text>
     </comment>
@@ -1009,21 +864,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F28")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B27" authorId="0" shapeId="0">
       <text>
         <r>
@@ -1034,7 +874,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[10].commingled== false", lastCell="B28", areas=["B27:B28","B114:B115"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[10].commingled==false", lastCell="B28", areas=["B27:B28","B114:B115"])</t>
         </r>
       </text>
     </comment>
@@ -1068,21 +908,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F30")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B29" authorId="0" shapeId="0">
       <text>
         <r>
@@ -1093,7 +918,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[11].commingled == false", lastCell="B30", areas=["B29:B30","B116:B117"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[11].commingled==false", lastCell="B30", areas=["B29:B30","B116:B117"])</t>
         </r>
       </text>
     </comment>
@@ -1127,21 +952,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A31" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F32")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B31" authorId="0" shapeId="0">
       <text>
         <r>
@@ -1152,7 +962,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[12].commingled== false", lastCell="B32", areas=["B31:B32","B118:B119"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[12].commingled==false", lastCell="B32", areas=["B31:B32","B118:B119"])</t>
         </r>
       </text>
     </comment>
@@ -1186,21 +996,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A33" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F34")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B33" authorId="0" shapeId="0">
       <text>
         <r>
@@ -1211,7 +1006,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[13].commingled== false", lastCell="B34", areas=["B33:B34","B120:B121"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[13].commingled==false", lastCell="B34", areas=["B33:B34","B120:B121"])</t>
         </r>
       </text>
     </comment>
@@ -1245,21 +1040,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A35" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F36")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B35" authorId="0" shapeId="0">
       <text>
         <r>
@@ -1270,7 +1050,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[14].commingled == false", lastCell="B36", areas=["B35:B36","B122:B123"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[14].commingled==false", lastCell="B36", areas=["B35:B36","B122:B123"])</t>
         </r>
       </text>
     </comment>
@@ -1304,21 +1084,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F38")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B37" authorId="0" shapeId="0">
       <text>
         <r>
@@ -1329,7 +1094,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[15].commingled == false", lastCell="B38", areas=["B37:B38","B124:B125"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[15].commingled==false", lastCell="B38", areas=["B37:B38","B124:B125"])</t>
         </r>
       </text>
     </comment>
@@ -1363,21 +1128,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A39" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:
-jx:area(lastCell="F40")</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B39" authorId="0" shapeId="0">
       <text>
         <r>
@@ -1388,7 +1138,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:if(condition="sheetThree.cargoTanks[16].commingled== false", lastCell="B40", areas=["B39:B40","B126:B127"])</t>
+          <t>jx:if(condition="sheetThree.cargoTanks[16].commingled==false", lastCell="B40", areas=["B39:B40","B126:B127"])</t>
         </r>
       </text>
     </comment>
@@ -5870,9 +5620,6 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5930,6 +5677,14 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" shrinkToFit="1"/>
@@ -6034,14 +5789,6 @@
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6215,6 +5962,9 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8003,7 +7753,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AS75"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
@@ -8117,13 +7867,13 @@
         <v>30</v>
       </c>
       <c r="C5" s="51"/>
-      <c r="D5" s="260" t="s">
+      <c r="D5" s="261" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="260"/>
-      <c r="F5" s="260"/>
-      <c r="G5" s="260"/>
-      <c r="H5" s="260"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
+      <c r="G5" s="261"/>
+      <c r="H5" s="261"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="52"/>
@@ -8141,13 +7891,13 @@
       <c r="U5" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="V5" s="326" t="s">
+      <c r="V5" s="325" t="s">
         <v>64</v>
       </c>
-      <c r="W5" s="326"/>
-      <c r="X5" s="326"/>
-      <c r="Y5" s="326"/>
-      <c r="Z5" s="326"/>
+      <c r="W5" s="325"/>
+      <c r="X5" s="325"/>
+      <c r="Y5" s="325"/>
+      <c r="Z5" s="325"/>
       <c r="AA5" s="48"/>
       <c r="AB5" s="56"/>
     </row>
@@ -8177,13 +7927,13 @@
       <c r="U6" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="V6" s="327" t="s">
+      <c r="V6" s="326" t="s">
         <v>65</v>
       </c>
-      <c r="W6" s="327"/>
-      <c r="X6" s="327"/>
-      <c r="Y6" s="327"/>
-      <c r="Z6" s="327"/>
+      <c r="W6" s="326"/>
+      <c r="X6" s="326"/>
+      <c r="Y6" s="326"/>
+      <c r="Z6" s="326"/>
       <c r="AA6" s="48"/>
       <c r="AB6" s="56"/>
     </row>
@@ -8221,13 +7971,13 @@
       <c r="U7" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="V7" s="327" t="s">
+      <c r="V7" s="326" t="s">
         <v>66</v>
       </c>
-      <c r="W7" s="327"/>
-      <c r="X7" s="327"/>
-      <c r="Y7" s="327"/>
-      <c r="Z7" s="327"/>
+      <c r="W7" s="326"/>
+      <c r="X7" s="326"/>
+      <c r="Y7" s="326"/>
+      <c r="Z7" s="326"/>
       <c r="AA7" s="48"/>
       <c r="AB7" s="56"/>
     </row>
@@ -8307,22 +8057,22 @@
       <c r="M10" s="60"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
-      <c r="P10" s="242" t="s">
+      <c r="P10" s="333" t="s">
         <v>58</v>
       </c>
-      <c r="Q10" s="242"/>
-      <c r="R10" s="242"/>
-      <c r="S10" s="242"/>
-      <c r="T10" s="242"/>
-      <c r="U10" s="242"/>
-      <c r="V10" s="242"/>
-      <c r="W10" s="242"/>
-      <c r="X10" s="244" t="s">
+      <c r="Q10" s="333"/>
+      <c r="R10" s="333"/>
+      <c r="S10" s="333"/>
+      <c r="T10" s="333"/>
+      <c r="U10" s="333"/>
+      <c r="V10" s="333"/>
+      <c r="W10" s="333"/>
+      <c r="X10" s="243" t="s">
         <v>67</v>
       </c>
-      <c r="Y10" s="244"/>
-      <c r="Z10" s="244"/>
-      <c r="AA10" s="244"/>
+      <c r="Y10" s="243"/>
+      <c r="Z10" s="243"/>
+      <c r="AA10" s="243"/>
       <c r="AB10" s="56"/>
     </row>
     <row r="11" spans="1:32" ht="17.25" customHeight="1">
@@ -8345,21 +8095,21 @@
       <c r="M11" s="63"/>
       <c r="N11" s="63"/>
       <c r="O11" s="64"/>
-      <c r="P11" s="243" t="s">
+      <c r="P11" s="242" t="s">
         <v>52</v>
       </c>
-      <c r="Q11" s="243"/>
-      <c r="R11" s="243"/>
-      <c r="S11" s="243"/>
-      <c r="T11" s="243"/>
-      <c r="U11" s="243"/>
-      <c r="V11" s="243"/>
-      <c r="W11" s="330" t="s">
+      <c r="Q11" s="242"/>
+      <c r="R11" s="242"/>
+      <c r="S11" s="242"/>
+      <c r="T11" s="242"/>
+      <c r="U11" s="242"/>
+      <c r="V11" s="242"/>
+      <c r="W11" s="329" t="s">
         <v>580</v>
       </c>
-      <c r="X11" s="330"/>
-      <c r="Y11" s="330"/>
-      <c r="Z11" s="330"/>
+      <c r="X11" s="329"/>
+      <c r="Y11" s="329"/>
+      <c r="Z11" s="329"/>
       <c r="AA11" s="65"/>
     </row>
     <row r="12" spans="1:32" s="65" customFormat="1" ht="17.25" customHeight="1">
@@ -8378,19 +8128,19 @@
       <c r="M12" s="67"/>
       <c r="N12" s="67"/>
       <c r="O12" s="67"/>
-      <c r="P12" s="329" t="s">
+      <c r="P12" s="328" t="s">
         <v>53</v>
       </c>
-      <c r="Q12" s="329"/>
-      <c r="R12" s="329"/>
-      <c r="S12" s="329"/>
-      <c r="T12" s="329"/>
-      <c r="U12" s="329"/>
-      <c r="V12" s="329"/>
-      <c r="W12" s="329"/>
-      <c r="X12" s="329"/>
-      <c r="Y12" s="329"/>
-      <c r="Z12" s="329"/>
+      <c r="Q12" s="328"/>
+      <c r="R12" s="328"/>
+      <c r="S12" s="328"/>
+      <c r="T12" s="328"/>
+      <c r="U12" s="328"/>
+      <c r="V12" s="328"/>
+      <c r="W12" s="328"/>
+      <c r="X12" s="328"/>
+      <c r="Y12" s="328"/>
+      <c r="Z12" s="328"/>
     </row>
     <row r="13" spans="1:32" s="65" customFormat="1" ht="17.25" customHeight="1">
       <c r="A13" s="66"/>
@@ -8451,8 +8201,8 @@
       <c r="G15" s="219" t="s">
         <v>262</v>
       </c>
-      <c r="H15" s="255"/>
-      <c r="I15" s="256"/>
+      <c r="H15" s="254"/>
+      <c r="I15" s="255"/>
       <c r="J15" s="75" t="s">
         <v>263</v>
       </c>
@@ -8460,8 +8210,8 @@
       <c r="L15" s="219" t="s">
         <v>264</v>
       </c>
-      <c r="M15" s="255"/>
-      <c r="N15" s="256"/>
+      <c r="M15" s="254"/>
+      <c r="N15" s="255"/>
       <c r="O15" s="75" t="s">
         <v>265</v>
       </c>
@@ -8469,12 +8219,12 @@
       <c r="Q15" s="77"/>
       <c r="R15" s="67"/>
       <c r="S15" s="67"/>
-      <c r="T15" s="324" t="s">
+      <c r="T15" s="323" t="s">
         <v>39</v>
       </c>
-      <c r="U15" s="324"/>
-      <c r="V15" s="324"/>
-      <c r="W15" s="324"/>
+      <c r="U15" s="323"/>
+      <c r="V15" s="323"/>
+      <c r="W15" s="323"/>
       <c r="X15" s="78"/>
       <c r="Y15" s="79"/>
       <c r="Z15" s="70"/>
@@ -8482,47 +8232,47 @@
     <row r="16" spans="1:32" s="65" customFormat="1" ht="12" customHeight="1">
       <c r="A16" s="80"/>
       <c r="B16" s="81"/>
-      <c r="C16" s="248" t="s">
+      <c r="C16" s="247" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="249"/>
-      <c r="E16" s="248" t="s">
+      <c r="D16" s="248"/>
+      <c r="E16" s="247" t="s">
         <v>109</v>
       </c>
-      <c r="F16" s="250"/>
-      <c r="G16" s="248" t="s">
+      <c r="F16" s="249"/>
+      <c r="G16" s="247" t="s">
         <v>137</v>
       </c>
-      <c r="H16" s="249"/>
-      <c r="I16" s="250"/>
-      <c r="J16" s="248" t="s">
+      <c r="H16" s="248"/>
+      <c r="I16" s="249"/>
+      <c r="J16" s="247" t="s">
         <v>165</v>
       </c>
-      <c r="K16" s="250"/>
-      <c r="L16" s="248" t="s">
+      <c r="K16" s="249"/>
+      <c r="L16" s="247" t="s">
         <v>193</v>
       </c>
-      <c r="M16" s="249"/>
-      <c r="N16" s="250"/>
-      <c r="O16" s="248" t="s">
+      <c r="M16" s="248"/>
+      <c r="N16" s="249"/>
+      <c r="O16" s="247" t="s">
         <v>221</v>
       </c>
-      <c r="P16" s="250"/>
+      <c r="P16" s="249"/>
       <c r="Q16" s="81"/>
       <c r="S16" s="67"/>
-      <c r="T16" s="331" t="s">
+      <c r="T16" s="330" t="s">
         <v>68</v>
       </c>
-      <c r="U16" s="331"/>
-      <c r="V16" s="331"/>
-      <c r="W16" s="331"/>
+      <c r="U16" s="330"/>
+      <c r="V16" s="330"/>
+      <c r="W16" s="330"/>
       <c r="X16" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="Y16" s="319" t="s">
+      <c r="Y16" s="318" t="s">
         <v>76</v>
       </c>
-      <c r="Z16" s="319"/>
+      <c r="Z16" s="318"/>
       <c r="AF16" s="100"/>
     </row>
     <row r="17" spans="1:45" s="65" customFormat="1" ht="12" customHeight="1">
@@ -8543,10 +8293,10 @@
       <c r="G17" s="216" t="s">
         <v>278</v>
       </c>
-      <c r="H17" s="281" t="s">
+      <c r="H17" s="282" t="s">
         <v>138</v>
       </c>
-      <c r="I17" s="282"/>
+      <c r="I17" s="283"/>
       <c r="J17" s="82" t="s">
         <v>281</v>
       </c>
@@ -8556,10 +8306,10 @@
       <c r="L17" s="216" t="s">
         <v>284</v>
       </c>
-      <c r="M17" s="281" t="s">
+      <c r="M17" s="282" t="s">
         <v>194</v>
       </c>
-      <c r="N17" s="282"/>
+      <c r="N17" s="283"/>
       <c r="O17" s="82" t="s">
         <v>287</v>
       </c>
@@ -8588,40 +8338,40 @@
     <row r="18" spans="1:45" s="65" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="80"/>
       <c r="B18" s="87"/>
-      <c r="C18" s="246" t="s">
+      <c r="C18" s="245" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="275"/>
-      <c r="E18" s="246" t="s">
+      <c r="D18" s="276"/>
+      <c r="E18" s="245" t="s">
         <v>111</v>
       </c>
-      <c r="F18" s="247"/>
-      <c r="G18" s="246" t="s">
+      <c r="F18" s="246"/>
+      <c r="G18" s="245" t="s">
         <v>139</v>
       </c>
-      <c r="H18" s="275"/>
-      <c r="I18" s="247"/>
-      <c r="J18" s="275" t="s">
+      <c r="H18" s="276"/>
+      <c r="I18" s="246"/>
+      <c r="J18" s="276" t="s">
         <v>167</v>
       </c>
-      <c r="K18" s="275"/>
-      <c r="L18" s="273" t="s">
+      <c r="K18" s="276"/>
+      <c r="L18" s="274" t="s">
         <v>195</v>
       </c>
-      <c r="M18" s="301"/>
-      <c r="N18" s="274"/>
-      <c r="O18" s="275" t="s">
+      <c r="M18" s="300"/>
+      <c r="N18" s="275"/>
+      <c r="O18" s="276" t="s">
         <v>223</v>
       </c>
-      <c r="P18" s="275"/>
-      <c r="Q18" s="300" t="s">
+      <c r="P18" s="276"/>
+      <c r="Q18" s="299" t="s">
         <v>557</v>
       </c>
       <c r="S18" s="67"/>
-      <c r="T18" s="328"/>
-      <c r="U18" s="328"/>
-      <c r="V18" s="328"/>
-      <c r="W18" s="328"/>
+      <c r="T18" s="327"/>
+      <c r="U18" s="327"/>
+      <c r="V18" s="327"/>
+      <c r="W18" s="327"/>
       <c r="X18" s="78"/>
       <c r="Y18" s="86"/>
       <c r="Z18" s="70"/>
@@ -8650,10 +8400,10 @@
       <c r="G19" s="222" t="s">
         <v>140</v>
       </c>
-      <c r="H19" s="251" t="s">
+      <c r="H19" s="250" t="s">
         <v>141</v>
       </c>
-      <c r="I19" s="252"/>
+      <c r="I19" s="251"/>
       <c r="J19" s="220" t="s">
         <v>168</v>
       </c>
@@ -8663,22 +8413,22 @@
       <c r="L19" s="220" t="s">
         <v>196</v>
       </c>
-      <c r="M19" s="251" t="s">
+      <c r="M19" s="250" t="s">
         <v>197</v>
       </c>
-      <c r="N19" s="252"/>
+      <c r="N19" s="251"/>
       <c r="O19" s="223" t="s">
         <v>224</v>
       </c>
       <c r="P19" s="221" t="s">
         <v>225</v>
       </c>
-      <c r="Q19" s="300"/>
+      <c r="Q19" s="299"/>
       <c r="S19" s="67"/>
-      <c r="T19" s="328"/>
-      <c r="U19" s="328"/>
-      <c r="V19" s="328"/>
-      <c r="W19" s="328"/>
+      <c r="T19" s="327"/>
+      <c r="U19" s="327"/>
+      <c r="V19" s="327"/>
+      <c r="W19" s="327"/>
       <c r="X19" s="78"/>
       <c r="Y19" s="86"/>
       <c r="Z19" s="70"/>
@@ -8701,18 +8451,18 @@
       <c r="C20" s="88" t="s">
         <v>273</v>
       </c>
-      <c r="D20" s="332" t="s">
+      <c r="D20" s="331" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="304"/>
-      <c r="F20" s="333"/>
+      <c r="E20" s="303"/>
+      <c r="F20" s="332"/>
       <c r="G20" s="217" t="s">
         <v>277</v>
       </c>
-      <c r="H20" s="283" t="s">
+      <c r="H20" s="284" t="s">
         <v>114</v>
       </c>
-      <c r="I20" s="284"/>
+      <c r="I20" s="285"/>
       <c r="J20" s="88" t="s">
         <v>279</v>
       </c>
@@ -8722,10 +8472,10 @@
       <c r="L20" s="91" t="s">
         <v>282</v>
       </c>
-      <c r="M20" s="302" t="s">
+      <c r="M20" s="301" t="s">
         <v>170</v>
       </c>
-      <c r="N20" s="303"/>
+      <c r="N20" s="302"/>
       <c r="O20" s="91" t="s">
         <v>285</v>
       </c>
@@ -8734,17 +8484,17 @@
       </c>
       <c r="Q20" s="229"/>
       <c r="S20" s="67"/>
-      <c r="T20" s="328"/>
-      <c r="U20" s="328"/>
-      <c r="V20" s="328"/>
-      <c r="W20" s="328"/>
+      <c r="T20" s="327"/>
+      <c r="U20" s="327"/>
+      <c r="V20" s="327"/>
+      <c r="W20" s="327"/>
       <c r="X20" s="78"/>
       <c r="Y20" s="86"/>
       <c r="Z20" s="70"/>
       <c r="AA20" s="80"/>
       <c r="AD20"/>
       <c r="AE20"/>
-      <c r="AF20" s="323" t="s">
+      <c r="AF20" s="322" t="s">
         <v>562</v>
       </c>
       <c r="AG20"/>
@@ -8752,30 +8502,30 @@
     <row r="21" spans="1:45" s="65" customFormat="1" ht="12" customHeight="1">
       <c r="A21" s="80"/>
       <c r="B21" s="335"/>
-      <c r="C21" s="246" t="s">
+      <c r="C21" s="245" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="275"/>
-      <c r="E21" s="275"/>
-      <c r="F21" s="247"/>
-      <c r="G21" s="246" t="s">
+      <c r="D21" s="276"/>
+      <c r="E21" s="276"/>
+      <c r="F21" s="246"/>
+      <c r="G21" s="245" t="s">
         <v>115</v>
       </c>
-      <c r="H21" s="275"/>
-      <c r="I21" s="247"/>
-      <c r="J21" s="273" t="s">
+      <c r="H21" s="276"/>
+      <c r="I21" s="246"/>
+      <c r="J21" s="274" t="s">
         <v>143</v>
       </c>
-      <c r="K21" s="274"/>
-      <c r="L21" s="273" t="s">
+      <c r="K21" s="275"/>
+      <c r="L21" s="274" t="s">
         <v>171</v>
       </c>
-      <c r="M21" s="301"/>
-      <c r="N21" s="274"/>
-      <c r="O21" s="273" t="s">
+      <c r="M21" s="300"/>
+      <c r="N21" s="275"/>
+      <c r="O21" s="274" t="s">
         <v>199</v>
       </c>
-      <c r="P21" s="274"/>
+      <c r="P21" s="275"/>
       <c r="Q21" s="230"/>
       <c r="S21" s="67"/>
       <c r="T21" s="67"/>
@@ -8788,7 +8538,7 @@
       <c r="AA21" s="80"/>
       <c r="AD21"/>
       <c r="AE21"/>
-      <c r="AF21" s="323"/>
+      <c r="AF21" s="322"/>
       <c r="AG21"/>
     </row>
     <row r="22" spans="1:45" s="65" customFormat="1" ht="12" customHeight="1">
@@ -8797,18 +8547,18 @@
       <c r="C22" s="224" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="279" t="s">
+      <c r="D22" s="280" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="279"/>
-      <c r="F22" s="280"/>
+      <c r="E22" s="280"/>
+      <c r="F22" s="281"/>
       <c r="G22" s="225" t="s">
         <v>116</v>
       </c>
-      <c r="H22" s="279" t="s">
+      <c r="H22" s="280" t="s">
         <v>117</v>
       </c>
-      <c r="I22" s="280"/>
+      <c r="I22" s="281"/>
       <c r="J22" s="226" t="s">
         <v>144</v>
       </c>
@@ -8818,10 +8568,10 @@
       <c r="L22" s="226" t="s">
         <v>172</v>
       </c>
-      <c r="M22" s="279" t="s">
+      <c r="M22" s="280" t="s">
         <v>173</v>
       </c>
-      <c r="N22" s="280"/>
+      <c r="N22" s="281"/>
       <c r="O22" s="228" t="s">
         <v>200</v>
       </c>
@@ -8860,10 +8610,10 @@
       <c r="G23" s="217" t="s">
         <v>280</v>
       </c>
-      <c r="H23" s="283" t="s">
+      <c r="H23" s="284" t="s">
         <v>146</v>
       </c>
-      <c r="I23" s="284"/>
+      <c r="I23" s="285"/>
       <c r="J23" s="88" t="s">
         <v>283</v>
       </c>
@@ -8873,10 +8623,10 @@
       <c r="L23" s="217" t="s">
         <v>286</v>
       </c>
-      <c r="M23" s="283" t="s">
+      <c r="M23" s="284" t="s">
         <v>202</v>
       </c>
-      <c r="N23" s="284"/>
+      <c r="N23" s="285"/>
       <c r="O23" s="88" t="s">
         <v>288</v>
       </c>
@@ -8906,42 +8656,42 @@
     <row r="24" spans="1:45" s="65" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="80"/>
       <c r="B24" s="81"/>
-      <c r="C24" s="246" t="s">
+      <c r="C24" s="245" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="275"/>
-      <c r="E24" s="246" t="s">
+      <c r="D24" s="276"/>
+      <c r="E24" s="245" t="s">
         <v>119</v>
       </c>
-      <c r="F24" s="275"/>
-      <c r="G24" s="276" t="s">
+      <c r="F24" s="276"/>
+      <c r="G24" s="277" t="s">
         <v>147</v>
       </c>
-      <c r="H24" s="277"/>
-      <c r="I24" s="278"/>
-      <c r="J24" s="246" t="s">
+      <c r="H24" s="278"/>
+      <c r="I24" s="279"/>
+      <c r="J24" s="245" t="s">
         <v>175</v>
       </c>
-      <c r="K24" s="275"/>
-      <c r="L24" s="276" t="s">
+      <c r="K24" s="276"/>
+      <c r="L24" s="277" t="s">
         <v>203</v>
       </c>
-      <c r="M24" s="277"/>
-      <c r="N24" s="278"/>
-      <c r="O24" s="246" t="s">
+      <c r="M24" s="278"/>
+      <c r="N24" s="279"/>
+      <c r="O24" s="245" t="s">
         <v>227</v>
       </c>
-      <c r="P24" s="275"/>
-      <c r="Q24" s="300" t="s">
+      <c r="P24" s="276"/>
+      <c r="Q24" s="299" t="s">
         <v>555</v>
       </c>
       <c r="S24" s="67"/>
-      <c r="T24" s="310" t="s">
+      <c r="T24" s="309" t="s">
         <v>250</v>
       </c>
-      <c r="U24" s="310"/>
-      <c r="V24" s="310"/>
-      <c r="W24" s="310"/>
+      <c r="U24" s="309"/>
+      <c r="V24" s="309"/>
+      <c r="W24" s="309"/>
       <c r="X24" s="78"/>
       <c r="Y24" s="95" t="s">
         <v>258</v>
@@ -8972,10 +8722,10 @@
       <c r="G25" s="222" t="s">
         <v>148</v>
       </c>
-      <c r="H25" s="253" t="s">
+      <c r="H25" s="252" t="s">
         <v>149</v>
       </c>
-      <c r="I25" s="254"/>
+      <c r="I25" s="253"/>
       <c r="J25" s="220" t="s">
         <v>176</v>
       </c>
@@ -8985,17 +8735,17 @@
       <c r="L25" s="220" t="s">
         <v>204</v>
       </c>
-      <c r="M25" s="298" t="s">
+      <c r="M25" s="297" t="s">
         <v>205</v>
       </c>
-      <c r="N25" s="299"/>
+      <c r="N25" s="298"/>
       <c r="O25" s="220" t="s">
         <v>228</v>
       </c>
       <c r="P25" s="221" t="s">
         <v>229</v>
       </c>
-      <c r="Q25" s="300"/>
+      <c r="Q25" s="299"/>
       <c r="S25" s="67"/>
       <c r="T25" s="67"/>
       <c r="U25" s="67"/>
@@ -9025,8 +8775,8 @@
       <c r="G26" s="218" t="s">
         <v>268</v>
       </c>
-      <c r="H26" s="285"/>
-      <c r="I26" s="286"/>
+      <c r="H26" s="257"/>
+      <c r="I26" s="258"/>
       <c r="J26" s="96" t="s">
         <v>269</v>
       </c>
@@ -9034,19 +8784,19 @@
       <c r="L26" s="218" t="s">
         <v>270</v>
       </c>
-      <c r="M26" s="285"/>
-      <c r="N26" s="286"/>
+      <c r="M26" s="257"/>
+      <c r="N26" s="258"/>
       <c r="O26" s="72" t="s">
         <v>271</v>
       </c>
       <c r="P26" s="99"/>
       <c r="Q26" s="81"/>
       <c r="S26" s="67"/>
-      <c r="T26" s="290" t="s">
+      <c r="T26" s="289" t="s">
         <v>40</v>
       </c>
-      <c r="U26" s="290"/>
-      <c r="V26" s="290"/>
+      <c r="U26" s="289"/>
+      <c r="V26" s="289"/>
       <c r="W26" s="70" t="s">
         <v>8</v>
       </c>
@@ -9065,40 +8815,40 @@
     <row r="27" spans="1:45" s="65" customFormat="1" ht="12" customHeight="1">
       <c r="A27" s="80"/>
       <c r="B27" s="71"/>
-      <c r="C27" s="248" t="s">
+      <c r="C27" s="247" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="249"/>
-      <c r="E27" s="248" t="s">
+      <c r="D27" s="248"/>
+      <c r="E27" s="247" t="s">
         <v>122</v>
       </c>
-      <c r="F27" s="249"/>
-      <c r="G27" s="248" t="s">
+      <c r="F27" s="248"/>
+      <c r="G27" s="247" t="s">
         <v>150</v>
       </c>
-      <c r="H27" s="249"/>
-      <c r="I27" s="250"/>
-      <c r="J27" s="248" t="s">
+      <c r="H27" s="248"/>
+      <c r="I27" s="249"/>
+      <c r="J27" s="247" t="s">
         <v>178</v>
       </c>
-      <c r="K27" s="249"/>
-      <c r="L27" s="248" t="s">
+      <c r="K27" s="248"/>
+      <c r="L27" s="247" t="s">
         <v>206</v>
       </c>
-      <c r="M27" s="249"/>
-      <c r="N27" s="250"/>
-      <c r="O27" s="248" t="s">
+      <c r="M27" s="248"/>
+      <c r="N27" s="249"/>
+      <c r="O27" s="247" t="s">
         <v>230</v>
       </c>
-      <c r="P27" s="250"/>
+      <c r="P27" s="249"/>
       <c r="Q27" s="100"/>
       <c r="R27" s="67"/>
       <c r="S27" s="69"/>
-      <c r="T27" s="290" t="s">
+      <c r="T27" s="289" t="s">
         <v>69</v>
       </c>
-      <c r="U27" s="290"/>
-      <c r="V27" s="290"/>
+      <c r="U27" s="289"/>
+      <c r="V27" s="289"/>
       <c r="W27" s="70" t="s">
         <v>8</v>
       </c>
@@ -9134,11 +8884,11 @@
       <c r="Q28" s="100"/>
       <c r="R28" s="67"/>
       <c r="S28" s="69"/>
-      <c r="T28" s="310" t="s">
+      <c r="T28" s="309" t="s">
         <v>42</v>
       </c>
-      <c r="U28" s="310"/>
-      <c r="V28" s="310"/>
+      <c r="U28" s="309"/>
+      <c r="V28" s="309"/>
       <c r="W28" s="70" t="s">
         <v>8</v>
       </c>
@@ -9257,12 +9007,12 @@
       <c r="Q31" s="63"/>
       <c r="R31" s="103"/>
       <c r="S31" s="107"/>
-      <c r="T31" s="324" t="s">
+      <c r="T31" s="323" t="s">
         <v>39</v>
       </c>
-      <c r="U31" s="324"/>
-      <c r="V31" s="324"/>
-      <c r="W31" s="324"/>
+      <c r="U31" s="323"/>
+      <c r="V31" s="323"/>
+      <c r="W31" s="323"/>
       <c r="X31" s="105"/>
       <c r="Y31" s="106"/>
       <c r="Z31" s="70"/>
@@ -9293,32 +9043,32 @@
       <c r="Q32" s="108"/>
       <c r="R32" s="108"/>
       <c r="S32" s="108"/>
-      <c r="T32" s="325" t="s">
+      <c r="T32" s="324" t="s">
         <v>77</v>
       </c>
-      <c r="U32" s="325"/>
-      <c r="V32" s="325"/>
-      <c r="W32" s="325"/>
+      <c r="U32" s="324"/>
+      <c r="V32" s="324"/>
+      <c r="W32" s="324"/>
       <c r="X32" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="Y32" s="319" t="s">
+      <c r="Y32" s="318" t="s">
         <v>78</v>
       </c>
-      <c r="Z32" s="319"/>
+      <c r="Z32" s="318"/>
       <c r="AD32"/>
       <c r="AE32"/>
       <c r="AF32"/>
       <c r="AG32"/>
       <c r="AH32"/>
       <c r="AI32"/>
-      <c r="AJ32" s="317"/>
-      <c r="AK32" s="317"/>
+      <c r="AJ32" s="316"/>
+      <c r="AK32" s="316"/>
       <c r="AL32" s="111"/>
       <c r="AM32" s="111"/>
       <c r="AN32" s="111"/>
-      <c r="AO32" s="317"/>
-      <c r="AP32" s="317"/>
+      <c r="AO32" s="316"/>
+      <c r="AP32" s="316"/>
       <c r="AQ32" s="111"/>
       <c r="AR32" s="111"/>
       <c r="AS32" s="111"/>
@@ -9337,8 +9087,8 @@
       <c r="G33" s="219" t="s">
         <v>291</v>
       </c>
-      <c r="H33" s="255"/>
-      <c r="I33" s="256"/>
+      <c r="H33" s="254"/>
+      <c r="I33" s="255"/>
       <c r="J33" s="213" t="s">
         <v>292</v>
       </c>
@@ -9346,8 +9096,8 @@
       <c r="L33" s="219" t="s">
         <v>293</v>
       </c>
-      <c r="M33" s="255"/>
-      <c r="N33" s="256"/>
+      <c r="M33" s="254"/>
+      <c r="N33" s="255"/>
       <c r="O33" s="213" t="s">
         <v>294</v>
       </c>
@@ -9369,46 +9119,46 @@
       <c r="AG33"/>
       <c r="AH33"/>
       <c r="AI33"/>
-      <c r="AJ33" s="316"/>
-      <c r="AK33" s="316"/>
-      <c r="AL33" s="316"/>
-      <c r="AM33" s="316"/>
-      <c r="AN33" s="316"/>
-      <c r="AO33" s="316"/>
-      <c r="AP33" s="316"/>
-      <c r="AQ33" s="316"/>
-      <c r="AR33" s="316"/>
-      <c r="AS33" s="316"/>
+      <c r="AJ33" s="315"/>
+      <c r="AK33" s="315"/>
+      <c r="AL33" s="315"/>
+      <c r="AM33" s="315"/>
+      <c r="AN33" s="315"/>
+      <c r="AO33" s="315"/>
+      <c r="AP33" s="315"/>
+      <c r="AQ33" s="315"/>
+      <c r="AR33" s="315"/>
+      <c r="AS33" s="315"/>
     </row>
     <row r="34" spans="1:45" s="65" customFormat="1" ht="12" customHeight="1">
       <c r="A34" s="114"/>
       <c r="B34" s="81"/>
-      <c r="C34" s="248" t="s">
+      <c r="C34" s="247" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="250"/>
-      <c r="E34" s="248" t="s">
+      <c r="D34" s="249"/>
+      <c r="E34" s="247" t="s">
         <v>123</v>
       </c>
-      <c r="F34" s="250"/>
-      <c r="G34" s="248" t="s">
+      <c r="F34" s="249"/>
+      <c r="G34" s="247" t="s">
         <v>151</v>
       </c>
-      <c r="H34" s="249"/>
-      <c r="I34" s="250"/>
-      <c r="J34" s="248" t="s">
+      <c r="H34" s="248"/>
+      <c r="I34" s="249"/>
+      <c r="J34" s="247" t="s">
         <v>179</v>
       </c>
-      <c r="K34" s="250"/>
-      <c r="L34" s="248" t="s">
+      <c r="K34" s="249"/>
+      <c r="L34" s="247" t="s">
         <v>207</v>
       </c>
-      <c r="M34" s="249"/>
-      <c r="N34" s="250"/>
-      <c r="O34" s="248" t="s">
+      <c r="M34" s="248"/>
+      <c r="N34" s="249"/>
+      <c r="O34" s="247" t="s">
         <v>231</v>
       </c>
-      <c r="P34" s="250"/>
+      <c r="P34" s="249"/>
       <c r="Q34" s="81"/>
       <c r="S34" s="112"/>
       <c r="T34" s="113"/>
@@ -9426,13 +9176,13 @@
       <c r="AG34"/>
       <c r="AH34"/>
       <c r="AI34"/>
-      <c r="AJ34" s="320"/>
-      <c r="AK34" s="320"/>
+      <c r="AJ34" s="319"/>
+      <c r="AK34" s="319"/>
       <c r="AL34" s="116"/>
       <c r="AM34" s="115"/>
       <c r="AN34" s="116"/>
-      <c r="AO34" s="320"/>
-      <c r="AP34" s="320"/>
+      <c r="AO34" s="319"/>
+      <c r="AP34" s="319"/>
       <c r="AQ34" s="116"/>
       <c r="AR34" s="115"/>
       <c r="AS34" s="116"/>
@@ -9455,10 +9205,10 @@
       <c r="G35" s="216" t="s">
         <v>297</v>
       </c>
-      <c r="H35" s="281" t="s">
+      <c r="H35" s="282" t="s">
         <v>152</v>
       </c>
-      <c r="I35" s="282"/>
+      <c r="I35" s="283"/>
       <c r="J35" s="216" t="s">
         <v>298</v>
       </c>
@@ -9468,10 +9218,10 @@
       <c r="L35" s="216" t="s">
         <v>299</v>
       </c>
-      <c r="M35" s="281" t="s">
+      <c r="M35" s="282" t="s">
         <v>208</v>
       </c>
-      <c r="N35" s="282"/>
+      <c r="N35" s="283"/>
       <c r="O35" s="216" t="s">
         <v>300</v>
       </c>
@@ -9500,47 +9250,47 @@
       <c r="AG35"/>
       <c r="AH35"/>
       <c r="AI35"/>
-      <c r="AJ35" s="316"/>
-      <c r="AK35" s="316"/>
-      <c r="AL35" s="316"/>
-      <c r="AM35" s="316"/>
-      <c r="AN35" s="316"/>
-      <c r="AO35" s="277"/>
-      <c r="AP35" s="277"/>
-      <c r="AQ35" s="277"/>
-      <c r="AR35" s="321"/>
-      <c r="AS35" s="321"/>
+      <c r="AJ35" s="315"/>
+      <c r="AK35" s="315"/>
+      <c r="AL35" s="315"/>
+      <c r="AM35" s="315"/>
+      <c r="AN35" s="315"/>
+      <c r="AO35" s="278"/>
+      <c r="AP35" s="278"/>
+      <c r="AQ35" s="278"/>
+      <c r="AR35" s="320"/>
+      <c r="AS35" s="320"/>
     </row>
     <row r="36" spans="1:45" s="65" customFormat="1" ht="12" customHeight="1">
       <c r="A36" s="114"/>
       <c r="B36" s="81"/>
-      <c r="C36" s="246" t="s">
+      <c r="C36" s="245" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="247"/>
-      <c r="E36" s="246" t="s">
+      <c r="D36" s="246"/>
+      <c r="E36" s="245" t="s">
         <v>125</v>
       </c>
-      <c r="F36" s="247"/>
-      <c r="G36" s="246" t="s">
+      <c r="F36" s="246"/>
+      <c r="G36" s="245" t="s">
         <v>153</v>
       </c>
-      <c r="H36" s="275"/>
-      <c r="I36" s="247"/>
-      <c r="J36" s="246" t="s">
+      <c r="H36" s="276"/>
+      <c r="I36" s="246"/>
+      <c r="J36" s="245" t="s">
         <v>181</v>
       </c>
-      <c r="K36" s="247"/>
-      <c r="L36" s="273" t="s">
+      <c r="K36" s="246"/>
+      <c r="L36" s="274" t="s">
         <v>209</v>
       </c>
-      <c r="M36" s="301"/>
-      <c r="N36" s="274"/>
-      <c r="O36" s="246" t="s">
+      <c r="M36" s="300"/>
+      <c r="N36" s="275"/>
+      <c r="O36" s="245" t="s">
         <v>233</v>
       </c>
-      <c r="P36" s="247"/>
-      <c r="Q36" s="300" t="s">
+      <c r="P36" s="246"/>
+      <c r="Q36" s="299" t="s">
         <v>558</v>
       </c>
       <c r="S36" s="112"/>
@@ -9590,10 +9340,10 @@
       <c r="G37" s="220" t="s">
         <v>154</v>
       </c>
-      <c r="H37" s="251" t="s">
+      <c r="H37" s="250" t="s">
         <v>155</v>
       </c>
-      <c r="I37" s="252"/>
+      <c r="I37" s="251"/>
       <c r="J37" s="220" t="s">
         <v>182</v>
       </c>
@@ -9603,17 +9353,17 @@
       <c r="L37" s="220" t="s">
         <v>210</v>
       </c>
-      <c r="M37" s="251" t="s">
+      <c r="M37" s="250" t="s">
         <v>211</v>
       </c>
-      <c r="N37" s="252"/>
+      <c r="N37" s="251"/>
       <c r="O37" s="223" t="s">
         <v>234</v>
       </c>
       <c r="P37" s="221" t="s">
         <v>235</v>
       </c>
-      <c r="Q37" s="300"/>
+      <c r="Q37" s="299"/>
       <c r="S37" s="122"/>
       <c r="T37" s="113"/>
       <c r="U37" s="113"/>
@@ -9632,14 +9382,14 @@
       <c r="AG37" s="233"/>
       <c r="AH37" s="233"/>
       <c r="AI37" s="233"/>
-      <c r="AJ37" s="318"/>
-      <c r="AK37" s="318"/>
+      <c r="AJ37" s="317"/>
+      <c r="AK37" s="317"/>
       <c r="AL37" s="116"/>
       <c r="AM37" s="93"/>
       <c r="AN37" s="117"/>
       <c r="AO37" s="93"/>
-      <c r="AP37" s="322"/>
-      <c r="AQ37" s="322"/>
+      <c r="AP37" s="321"/>
+      <c r="AQ37" s="321"/>
       <c r="AR37" s="93"/>
       <c r="AS37" s="116"/>
     </row>
@@ -9651,18 +9401,18 @@
       <c r="C38" s="214" t="s">
         <v>301</v>
       </c>
-      <c r="D38" s="304" t="s">
+      <c r="D38" s="303" t="s">
         <v>100</v>
       </c>
-      <c r="E38" s="304"/>
-      <c r="F38" s="305"/>
+      <c r="E38" s="303"/>
+      <c r="F38" s="304"/>
       <c r="G38" s="217" t="s">
         <v>302</v>
       </c>
-      <c r="H38" s="283" t="s">
+      <c r="H38" s="284" t="s">
         <v>128</v>
       </c>
-      <c r="I38" s="284"/>
+      <c r="I38" s="285"/>
       <c r="J38" s="214" t="s">
         <v>303</v>
       </c>
@@ -9672,10 +9422,10 @@
       <c r="L38" s="91" t="s">
         <v>304</v>
       </c>
-      <c r="M38" s="302" t="s">
+      <c r="M38" s="301" t="s">
         <v>184</v>
       </c>
-      <c r="N38" s="303"/>
+      <c r="N38" s="302"/>
       <c r="O38" s="91" t="s">
         <v>305</v>
       </c>
@@ -9691,50 +9441,50 @@
       <c r="X38" s="67"/>
       <c r="Y38" s="123"/>
       <c r="Z38" s="67"/>
-      <c r="AF38" s="323" t="s">
+      <c r="AF38" s="322" t="s">
         <v>569</v>
       </c>
       <c r="AG38" s="232"/>
       <c r="AH38" s="232"/>
       <c r="AI38" s="232"/>
-      <c r="AJ38" s="316"/>
-      <c r="AK38" s="316"/>
-      <c r="AL38" s="316"/>
-      <c r="AM38" s="277"/>
-      <c r="AN38" s="277"/>
-      <c r="AO38" s="277"/>
-      <c r="AP38" s="277"/>
-      <c r="AQ38" s="277"/>
-      <c r="AR38" s="277"/>
-      <c r="AS38" s="277"/>
+      <c r="AJ38" s="315"/>
+      <c r="AK38" s="315"/>
+      <c r="AL38" s="315"/>
+      <c r="AM38" s="278"/>
+      <c r="AN38" s="278"/>
+      <c r="AO38" s="278"/>
+      <c r="AP38" s="278"/>
+      <c r="AQ38" s="278"/>
+      <c r="AR38" s="278"/>
+      <c r="AS38" s="278"/>
     </row>
     <row r="39" spans="1:45" s="65" customFormat="1" ht="12" customHeight="1">
       <c r="A39" s="114"/>
       <c r="B39" s="335"/>
-      <c r="C39" s="246" t="s">
+      <c r="C39" s="245" t="s">
         <v>101</v>
       </c>
-      <c r="D39" s="275"/>
-      <c r="E39" s="275"/>
-      <c r="F39" s="247"/>
-      <c r="G39" s="246" t="s">
+      <c r="D39" s="276"/>
+      <c r="E39" s="276"/>
+      <c r="F39" s="246"/>
+      <c r="G39" s="245" t="s">
         <v>129</v>
       </c>
-      <c r="H39" s="275"/>
-      <c r="I39" s="247"/>
-      <c r="J39" s="273" t="s">
+      <c r="H39" s="276"/>
+      <c r="I39" s="246"/>
+      <c r="J39" s="274" t="s">
         <v>157</v>
       </c>
-      <c r="K39" s="274"/>
-      <c r="L39" s="273" t="s">
+      <c r="K39" s="275"/>
+      <c r="L39" s="274" t="s">
         <v>185</v>
       </c>
-      <c r="M39" s="301"/>
-      <c r="N39" s="274"/>
-      <c r="O39" s="273" t="s">
+      <c r="M39" s="300"/>
+      <c r="N39" s="275"/>
+      <c r="O39" s="274" t="s">
         <v>213</v>
       </c>
-      <c r="P39" s="274"/>
+      <c r="P39" s="275"/>
       <c r="Q39" s="230"/>
       <c r="S39" s="122"/>
       <c r="T39" s="69" t="s">
@@ -9746,7 +9496,7 @@
       <c r="X39" s="67"/>
       <c r="Y39" s="123"/>
       <c r="Z39" s="70"/>
-      <c r="AF39" s="323"/>
+      <c r="AF39" s="322"/>
       <c r="AG39" s="234"/>
       <c r="AH39" s="234"/>
       <c r="AI39" s="121"/>
@@ -9767,18 +9517,18 @@
       <c r="C40" s="224" t="s">
         <v>102</v>
       </c>
-      <c r="D40" s="279" t="s">
+      <c r="D40" s="280" t="s">
         <v>103</v>
       </c>
-      <c r="E40" s="279"/>
-      <c r="F40" s="280"/>
+      <c r="E40" s="280"/>
+      <c r="F40" s="281"/>
       <c r="G40" s="225" t="s">
         <v>130</v>
       </c>
-      <c r="H40" s="279" t="s">
+      <c r="H40" s="280" t="s">
         <v>131</v>
       </c>
-      <c r="I40" s="280"/>
+      <c r="I40" s="281"/>
       <c r="J40" s="226" t="s">
         <v>158</v>
       </c>
@@ -9788,10 +9538,10 @@
       <c r="L40" s="226" t="s">
         <v>186</v>
       </c>
-      <c r="M40" s="279" t="s">
+      <c r="M40" s="280" t="s">
         <v>187</v>
       </c>
-      <c r="N40" s="280"/>
+      <c r="N40" s="281"/>
       <c r="O40" s="228" t="s">
         <v>214</v>
       </c>
@@ -9800,12 +9550,12 @@
       </c>
       <c r="Q40" s="94"/>
       <c r="S40" s="63"/>
-      <c r="T40" s="310" t="s">
+      <c r="T40" s="309" t="s">
         <v>250</v>
       </c>
-      <c r="U40" s="310"/>
-      <c r="V40" s="310"/>
-      <c r="W40" s="310"/>
+      <c r="U40" s="309"/>
+      <c r="V40" s="309"/>
+      <c r="W40" s="309"/>
       <c r="X40" s="78"/>
       <c r="Y40" s="124" t="s">
         <v>79</v>
@@ -9815,13 +9565,13 @@
       <c r="AG40" s="116"/>
       <c r="AH40" s="234"/>
       <c r="AI40" s="233"/>
-      <c r="AJ40" s="318"/>
-      <c r="AK40" s="318"/>
+      <c r="AJ40" s="317"/>
+      <c r="AK40" s="317"/>
       <c r="AL40" s="116"/>
       <c r="AM40" s="93"/>
       <c r="AN40" s="116"/>
-      <c r="AO40" s="318"/>
-      <c r="AP40" s="318"/>
+      <c r="AO40" s="317"/>
+      <c r="AP40" s="317"/>
       <c r="AQ40" s="116"/>
       <c r="AR40" s="93"/>
       <c r="AS40" s="116"/>
@@ -9844,10 +9594,10 @@
       <c r="G41" s="217" t="s">
         <v>308</v>
       </c>
-      <c r="H41" s="283" t="s">
+      <c r="H41" s="284" t="s">
         <v>160</v>
       </c>
-      <c r="I41" s="284"/>
+      <c r="I41" s="285"/>
       <c r="J41" s="214" t="s">
         <v>309</v>
       </c>
@@ -9857,10 +9607,10 @@
       <c r="L41" s="217" t="s">
         <v>310</v>
       </c>
-      <c r="M41" s="283" t="s">
+      <c r="M41" s="284" t="s">
         <v>216</v>
       </c>
-      <c r="N41" s="284"/>
+      <c r="N41" s="285"/>
       <c r="O41" s="214" t="s">
         <v>311</v>
       </c>
@@ -9882,55 +9632,55 @@
       <c r="AG41" s="231"/>
       <c r="AH41" s="231"/>
       <c r="AI41" s="231"/>
-      <c r="AJ41" s="277"/>
-      <c r="AK41" s="277"/>
-      <c r="AL41" s="277"/>
-      <c r="AM41" s="316"/>
-      <c r="AN41" s="316"/>
-      <c r="AO41" s="277"/>
-      <c r="AP41" s="277"/>
-      <c r="AQ41" s="277"/>
-      <c r="AR41" s="277"/>
-      <c r="AS41" s="277"/>
+      <c r="AJ41" s="278"/>
+      <c r="AK41" s="278"/>
+      <c r="AL41" s="278"/>
+      <c r="AM41" s="315"/>
+      <c r="AN41" s="315"/>
+      <c r="AO41" s="278"/>
+      <c r="AP41" s="278"/>
+      <c r="AQ41" s="278"/>
+      <c r="AR41" s="278"/>
+      <c r="AS41" s="278"/>
     </row>
     <row r="42" spans="1:45" s="65" customFormat="1" ht="12" customHeight="1">
       <c r="A42" s="114"/>
       <c r="B42" s="81"/>
-      <c r="C42" s="246" t="s">
+      <c r="C42" s="245" t="s">
         <v>105</v>
       </c>
-      <c r="D42" s="247"/>
-      <c r="E42" s="246" t="s">
+      <c r="D42" s="246"/>
+      <c r="E42" s="245" t="s">
         <v>133</v>
       </c>
-      <c r="F42" s="247"/>
-      <c r="G42" s="276" t="s">
+      <c r="F42" s="246"/>
+      <c r="G42" s="277" t="s">
         <v>161</v>
       </c>
-      <c r="H42" s="277"/>
-      <c r="I42" s="278"/>
-      <c r="J42" s="246" t="s">
+      <c r="H42" s="278"/>
+      <c r="I42" s="279"/>
+      <c r="J42" s="245" t="s">
         <v>189</v>
       </c>
-      <c r="K42" s="247"/>
-      <c r="L42" s="276" t="s">
+      <c r="K42" s="246"/>
+      <c r="L42" s="277" t="s">
         <v>217</v>
       </c>
-      <c r="M42" s="277"/>
-      <c r="N42" s="278"/>
-      <c r="O42" s="246" t="s">
+      <c r="M42" s="278"/>
+      <c r="N42" s="279"/>
+      <c r="O42" s="245" t="s">
         <v>237</v>
       </c>
-      <c r="P42" s="247"/>
-      <c r="Q42" s="300" t="s">
+      <c r="P42" s="246"/>
+      <c r="Q42" s="299" t="s">
         <v>556</v>
       </c>
       <c r="S42" s="67"/>
-      <c r="T42" s="290" t="s">
+      <c r="T42" s="289" t="s">
         <v>40</v>
       </c>
-      <c r="U42" s="290"/>
-      <c r="V42" s="290"/>
+      <c r="U42" s="289"/>
+      <c r="V42" s="289"/>
       <c r="W42" s="70" t="s">
         <v>8</v>
       </c>
@@ -9972,10 +9722,10 @@
       <c r="G43" s="220" t="s">
         <v>162</v>
       </c>
-      <c r="H43" s="253" t="s">
+      <c r="H43" s="252" t="s">
         <v>163</v>
       </c>
-      <c r="I43" s="254"/>
+      <c r="I43" s="253"/>
       <c r="J43" s="220" t="s">
         <v>190</v>
       </c>
@@ -9985,23 +9735,23 @@
       <c r="L43" s="220" t="s">
         <v>218</v>
       </c>
-      <c r="M43" s="251" t="s">
+      <c r="M43" s="250" t="s">
         <v>219</v>
       </c>
-      <c r="N43" s="252"/>
+      <c r="N43" s="251"/>
       <c r="O43" s="220" t="s">
         <v>238</v>
       </c>
       <c r="P43" s="221" t="s">
         <v>239</v>
       </c>
-      <c r="Q43" s="300"/>
+      <c r="Q43" s="299"/>
       <c r="S43" s="67"/>
-      <c r="T43" s="290" t="s">
+      <c r="T43" s="289" t="s">
         <v>69</v>
       </c>
-      <c r="U43" s="290"/>
-      <c r="V43" s="290"/>
+      <c r="U43" s="289"/>
+      <c r="V43" s="289"/>
       <c r="W43" s="70" t="s">
         <v>8</v>
       </c>
@@ -10014,13 +9764,13 @@
       <c r="AG43" s="235"/>
       <c r="AH43" s="235"/>
       <c r="AI43" s="235"/>
-      <c r="AJ43" s="317"/>
-      <c r="AK43" s="317"/>
+      <c r="AJ43" s="316"/>
+      <c r="AK43" s="316"/>
       <c r="AL43" s="111"/>
       <c r="AM43" s="111"/>
       <c r="AN43" s="111"/>
-      <c r="AO43" s="317"/>
-      <c r="AP43" s="317"/>
+      <c r="AO43" s="316"/>
+      <c r="AP43" s="316"/>
       <c r="AQ43" s="111"/>
       <c r="AR43" s="111"/>
       <c r="AS43" s="111"/>
@@ -10039,8 +9789,8 @@
       <c r="G44" s="219" t="s">
         <v>314</v>
       </c>
-      <c r="H44" s="255"/>
-      <c r="I44" s="256"/>
+      <c r="H44" s="254"/>
+      <c r="I44" s="255"/>
       <c r="J44" s="96" t="s">
         <v>315</v>
       </c>
@@ -10048,19 +9798,19 @@
       <c r="L44" s="219" t="s">
         <v>316</v>
       </c>
-      <c r="M44" s="255"/>
-      <c r="N44" s="256"/>
+      <c r="M44" s="254"/>
+      <c r="N44" s="255"/>
       <c r="O44" s="72" t="s">
         <v>317</v>
       </c>
       <c r="P44" s="99"/>
       <c r="Q44" s="81"/>
       <c r="S44" s="67"/>
-      <c r="T44" s="310" t="s">
+      <c r="T44" s="309" t="s">
         <v>42</v>
       </c>
-      <c r="U44" s="310"/>
-      <c r="V44" s="310"/>
+      <c r="U44" s="309"/>
+      <c r="V44" s="309"/>
       <c r="W44" s="70" t="s">
         <v>8</v>
       </c>
@@ -10076,46 +9826,46 @@
       <c r="AG44" s="232"/>
       <c r="AH44" s="232"/>
       <c r="AI44" s="232"/>
-      <c r="AJ44" s="316"/>
-      <c r="AK44" s="316"/>
-      <c r="AL44" s="316"/>
-      <c r="AM44" s="316"/>
-      <c r="AN44" s="316"/>
-      <c r="AO44" s="316"/>
-      <c r="AP44" s="316"/>
-      <c r="AQ44" s="316"/>
-      <c r="AR44" s="316"/>
-      <c r="AS44" s="316"/>
+      <c r="AJ44" s="315"/>
+      <c r="AK44" s="315"/>
+      <c r="AL44" s="315"/>
+      <c r="AM44" s="315"/>
+      <c r="AN44" s="315"/>
+      <c r="AO44" s="315"/>
+      <c r="AP44" s="315"/>
+      <c r="AQ44" s="315"/>
+      <c r="AR44" s="315"/>
+      <c r="AS44" s="315"/>
     </row>
     <row r="45" spans="1:45" s="65" customFormat="1" ht="12" customHeight="1">
       <c r="A45" s="80"/>
       <c r="B45" s="71"/>
-      <c r="C45" s="248" t="s">
+      <c r="C45" s="247" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="250"/>
-      <c r="E45" s="248" t="s">
+      <c r="D45" s="249"/>
+      <c r="E45" s="247" t="s">
         <v>136</v>
       </c>
-      <c r="F45" s="250"/>
-      <c r="G45" s="248" t="s">
+      <c r="F45" s="249"/>
+      <c r="G45" s="247" t="s">
         <v>164</v>
       </c>
-      <c r="H45" s="249"/>
-      <c r="I45" s="250"/>
-      <c r="J45" s="248" t="s">
+      <c r="H45" s="248"/>
+      <c r="I45" s="249"/>
+      <c r="J45" s="247" t="s">
         <v>192</v>
       </c>
-      <c r="K45" s="250"/>
-      <c r="L45" s="248" t="s">
+      <c r="K45" s="249"/>
+      <c r="L45" s="247" t="s">
         <v>220</v>
       </c>
-      <c r="M45" s="249"/>
-      <c r="N45" s="250"/>
-      <c r="O45" s="248" t="s">
+      <c r="M45" s="248"/>
+      <c r="N45" s="249"/>
+      <c r="O45" s="247" t="s">
         <v>318</v>
       </c>
-      <c r="P45" s="250"/>
+      <c r="P45" s="249"/>
       <c r="Q45" s="100"/>
       <c r="R45" s="67"/>
       <c r="S45" s="69"/>
@@ -10130,18 +9880,18 @@
     <row r="46" spans="1:45" ht="17.25" customHeight="1">
       <c r="A46" s="56"/>
       <c r="B46" s="127"/>
-      <c r="C46" s="257"/>
-      <c r="D46" s="257"/>
-      <c r="E46" s="257"/>
-      <c r="F46" s="257"/>
-      <c r="G46" s="257"/>
-      <c r="H46" s="257"/>
-      <c r="I46" s="257"/>
-      <c r="J46" s="257"/>
-      <c r="K46" s="257"/>
-      <c r="L46" s="257"/>
-      <c r="M46" s="257"/>
-      <c r="N46" s="257"/>
+      <c r="C46" s="256"/>
+      <c r="D46" s="256"/>
+      <c r="E46" s="256"/>
+      <c r="F46" s="256"/>
+      <c r="G46" s="256"/>
+      <c r="H46" s="256"/>
+      <c r="I46" s="256"/>
+      <c r="J46" s="256"/>
+      <c r="K46" s="256"/>
+      <c r="L46" s="256"/>
+      <c r="M46" s="256"/>
+      <c r="N46" s="256"/>
       <c r="O46" s="109"/>
       <c r="P46" s="108"/>
       <c r="Q46" s="108"/>
@@ -10198,20 +9948,20 @@
       <c r="F48" s="129"/>
       <c r="G48" s="129"/>
       <c r="H48" s="129"/>
-      <c r="I48" s="291"/>
-      <c r="J48" s="291"/>
-      <c r="K48" s="291"/>
-      <c r="L48" s="291"/>
-      <c r="M48" s="261" t="s">
+      <c r="I48" s="290"/>
+      <c r="J48" s="290"/>
+      <c r="K48" s="290"/>
+      <c r="L48" s="290"/>
+      <c r="M48" s="262" t="s">
         <v>15</v>
       </c>
-      <c r="N48" s="262"/>
-      <c r="O48" s="262"/>
-      <c r="P48" s="262"/>
-      <c r="Q48" s="262"/>
-      <c r="R48" s="262"/>
-      <c r="S48" s="262"/>
-      <c r="T48" s="263"/>
+      <c r="N48" s="263"/>
+      <c r="O48" s="263"/>
+      <c r="P48" s="263"/>
+      <c r="Q48" s="263"/>
+      <c r="R48" s="263"/>
+      <c r="S48" s="263"/>
+      <c r="T48" s="264"/>
       <c r="U48" s="132"/>
       <c r="V48" s="132"/>
       <c r="W48" s="132"/>
@@ -10232,22 +9982,22 @@
       <c r="F49" s="135"/>
       <c r="G49" s="135"/>
       <c r="H49" s="136"/>
-      <c r="I49" s="245" t="s">
+      <c r="I49" s="244" t="s">
         <v>252</v>
       </c>
-      <c r="J49" s="245"/>
-      <c r="K49" s="245"/>
-      <c r="L49" s="245"/>
-      <c r="M49" s="264" t="s">
+      <c r="J49" s="244"/>
+      <c r="K49" s="244"/>
+      <c r="L49" s="244"/>
+      <c r="M49" s="265" t="s">
         <v>259</v>
       </c>
-      <c r="N49" s="265"/>
-      <c r="O49" s="265"/>
-      <c r="P49" s="265"/>
-      <c r="Q49" s="265"/>
-      <c r="R49" s="265"/>
-      <c r="S49" s="265"/>
-      <c r="T49" s="266"/>
+      <c r="N49" s="266"/>
+      <c r="O49" s="266"/>
+      <c r="P49" s="266"/>
+      <c r="Q49" s="266"/>
+      <c r="R49" s="266"/>
+      <c r="S49" s="266"/>
+      <c r="T49" s="267"/>
       <c r="U49" s="132"/>
       <c r="V49" s="132"/>
       <c r="W49" s="132"/>
@@ -10268,20 +10018,20 @@
       <c r="F50" s="135"/>
       <c r="G50" s="135"/>
       <c r="H50" s="136"/>
-      <c r="I50" s="245" t="s">
+      <c r="I50" s="244" t="s">
         <v>253</v>
       </c>
-      <c r="J50" s="245"/>
-      <c r="K50" s="245"/>
-      <c r="L50" s="245"/>
-      <c r="M50" s="267"/>
-      <c r="N50" s="268"/>
-      <c r="O50" s="268"/>
-      <c r="P50" s="268"/>
-      <c r="Q50" s="268"/>
-      <c r="R50" s="268"/>
-      <c r="S50" s="268"/>
-      <c r="T50" s="269"/>
+      <c r="J50" s="244"/>
+      <c r="K50" s="244"/>
+      <c r="L50" s="244"/>
+      <c r="M50" s="268"/>
+      <c r="N50" s="269"/>
+      <c r="O50" s="269"/>
+      <c r="P50" s="269"/>
+      <c r="Q50" s="269"/>
+      <c r="R50" s="269"/>
+      <c r="S50" s="269"/>
+      <c r="T50" s="270"/>
       <c r="U50" s="133"/>
       <c r="V50" s="132"/>
       <c r="W50" s="132"/>
@@ -10302,20 +10052,20 @@
       <c r="F51" s="135"/>
       <c r="G51" s="135"/>
       <c r="H51" s="136"/>
-      <c r="I51" s="245" t="s">
+      <c r="I51" s="244" t="s">
         <v>256</v>
       </c>
-      <c r="J51" s="245"/>
-      <c r="K51" s="245"/>
-      <c r="L51" s="245"/>
-      <c r="M51" s="267"/>
-      <c r="N51" s="268"/>
-      <c r="O51" s="268"/>
-      <c r="P51" s="268"/>
-      <c r="Q51" s="268"/>
-      <c r="R51" s="268"/>
-      <c r="S51" s="268"/>
-      <c r="T51" s="269"/>
+      <c r="J51" s="244"/>
+      <c r="K51" s="244"/>
+      <c r="L51" s="244"/>
+      <c r="M51" s="268"/>
+      <c r="N51" s="269"/>
+      <c r="O51" s="269"/>
+      <c r="P51" s="269"/>
+      <c r="Q51" s="269"/>
+      <c r="R51" s="269"/>
+      <c r="S51" s="269"/>
+      <c r="T51" s="270"/>
       <c r="U51" s="133"/>
       <c r="V51" s="132"/>
       <c r="W51" s="132"/>
@@ -10336,20 +10086,20 @@
       <c r="F52" s="135"/>
       <c r="G52" s="135"/>
       <c r="H52" s="136"/>
-      <c r="I52" s="245" t="s">
+      <c r="I52" s="244" t="s">
         <v>255</v>
       </c>
-      <c r="J52" s="245"/>
-      <c r="K52" s="245"/>
-      <c r="L52" s="245"/>
-      <c r="M52" s="267"/>
-      <c r="N52" s="268"/>
-      <c r="O52" s="268"/>
-      <c r="P52" s="268"/>
-      <c r="Q52" s="268"/>
-      <c r="R52" s="268"/>
-      <c r="S52" s="268"/>
-      <c r="T52" s="269"/>
+      <c r="J52" s="244"/>
+      <c r="K52" s="244"/>
+      <c r="L52" s="244"/>
+      <c r="M52" s="268"/>
+      <c r="N52" s="269"/>
+      <c r="O52" s="269"/>
+      <c r="P52" s="269"/>
+      <c r="Q52" s="269"/>
+      <c r="R52" s="269"/>
+      <c r="S52" s="269"/>
+      <c r="T52" s="270"/>
       <c r="U52" s="133"/>
       <c r="V52" s="132"/>
       <c r="W52" s="132"/>
@@ -10370,20 +10120,20 @@
       <c r="F53" s="135"/>
       <c r="G53" s="135"/>
       <c r="H53" s="136"/>
-      <c r="I53" s="245" t="s">
+      <c r="I53" s="244" t="s">
         <v>254</v>
       </c>
-      <c r="J53" s="245"/>
-      <c r="K53" s="245"/>
-      <c r="L53" s="245"/>
-      <c r="M53" s="267"/>
-      <c r="N53" s="268"/>
-      <c r="O53" s="268"/>
-      <c r="P53" s="268"/>
-      <c r="Q53" s="268"/>
-      <c r="R53" s="268"/>
-      <c r="S53" s="268"/>
-      <c r="T53" s="269"/>
+      <c r="J53" s="244"/>
+      <c r="K53" s="244"/>
+      <c r="L53" s="244"/>
+      <c r="M53" s="268"/>
+      <c r="N53" s="269"/>
+      <c r="O53" s="269"/>
+      <c r="P53" s="269"/>
+      <c r="Q53" s="269"/>
+      <c r="R53" s="269"/>
+      <c r="S53" s="269"/>
+      <c r="T53" s="270"/>
       <c r="U53" s="133"/>
       <c r="V53" s="132"/>
       <c r="W53" s="132"/>
@@ -10395,29 +10145,29 @@
     </row>
     <row r="54" spans="1:30" ht="13.2" customHeight="1">
       <c r="A54" s="131"/>
-      <c r="B54" s="287" t="s">
+      <c r="B54" s="286" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="288"/>
-      <c r="D54" s="288"/>
-      <c r="E54" s="288"/>
-      <c r="F54" s="288"/>
-      <c r="G54" s="288"/>
-      <c r="H54" s="289"/>
-      <c r="I54" s="296" t="s">
+      <c r="C54" s="287"/>
+      <c r="D54" s="287"/>
+      <c r="E54" s="287"/>
+      <c r="F54" s="287"/>
+      <c r="G54" s="287"/>
+      <c r="H54" s="288"/>
+      <c r="I54" s="295" t="s">
         <v>257</v>
       </c>
-      <c r="J54" s="296"/>
-      <c r="K54" s="296"/>
-      <c r="L54" s="296"/>
-      <c r="M54" s="267"/>
-      <c r="N54" s="268"/>
-      <c r="O54" s="268"/>
-      <c r="P54" s="268"/>
-      <c r="Q54" s="268"/>
-      <c r="R54" s="268"/>
-      <c r="S54" s="268"/>
-      <c r="T54" s="269"/>
+      <c r="J54" s="295"/>
+      <c r="K54" s="295"/>
+      <c r="L54" s="295"/>
+      <c r="M54" s="268"/>
+      <c r="N54" s="269"/>
+      <c r="O54" s="269"/>
+      <c r="P54" s="269"/>
+      <c r="Q54" s="269"/>
+      <c r="R54" s="269"/>
+      <c r="S54" s="269"/>
+      <c r="T54" s="270"/>
       <c r="U54" s="133"/>
       <c r="V54" s="132"/>
       <c r="W54" s="132"/>
@@ -10440,18 +10190,18 @@
       <c r="F55" s="139"/>
       <c r="G55" s="139"/>
       <c r="H55" s="140"/>
-      <c r="I55" s="296"/>
-      <c r="J55" s="296"/>
-      <c r="K55" s="296"/>
-      <c r="L55" s="296"/>
-      <c r="M55" s="267"/>
-      <c r="N55" s="268"/>
-      <c r="O55" s="268"/>
-      <c r="P55" s="268"/>
-      <c r="Q55" s="268"/>
-      <c r="R55" s="268"/>
-      <c r="S55" s="268"/>
-      <c r="T55" s="269"/>
+      <c r="I55" s="295"/>
+      <c r="J55" s="295"/>
+      <c r="K55" s="295"/>
+      <c r="L55" s="295"/>
+      <c r="M55" s="268"/>
+      <c r="N55" s="269"/>
+      <c r="O55" s="269"/>
+      <c r="P55" s="269"/>
+      <c r="Q55" s="269"/>
+      <c r="R55" s="269"/>
+      <c r="S55" s="269"/>
+      <c r="T55" s="270"/>
       <c r="U55" s="133"/>
       <c r="V55" s="132"/>
       <c r="W55" s="132"/>
@@ -10474,18 +10224,18 @@
       <c r="F56" s="139"/>
       <c r="G56" s="139"/>
       <c r="H56" s="140"/>
-      <c r="I56" s="296"/>
-      <c r="J56" s="296"/>
-      <c r="K56" s="296"/>
-      <c r="L56" s="296"/>
-      <c r="M56" s="267"/>
-      <c r="N56" s="268"/>
-      <c r="O56" s="268"/>
-      <c r="P56" s="268"/>
-      <c r="Q56" s="268"/>
-      <c r="R56" s="268"/>
-      <c r="S56" s="268"/>
-      <c r="T56" s="269"/>
+      <c r="I56" s="295"/>
+      <c r="J56" s="295"/>
+      <c r="K56" s="295"/>
+      <c r="L56" s="295"/>
+      <c r="M56" s="268"/>
+      <c r="N56" s="269"/>
+      <c r="O56" s="269"/>
+      <c r="P56" s="269"/>
+      <c r="Q56" s="269"/>
+      <c r="R56" s="269"/>
+      <c r="S56" s="269"/>
+      <c r="T56" s="270"/>
       <c r="U56" s="133"/>
       <c r="V56" s="132"/>
       <c r="W56" s="132"/>
@@ -10508,18 +10258,18 @@
       <c r="F57" s="139"/>
       <c r="G57" s="139"/>
       <c r="H57" s="140"/>
-      <c r="I57" s="296"/>
-      <c r="J57" s="296"/>
-      <c r="K57" s="296"/>
-      <c r="L57" s="296"/>
-      <c r="M57" s="267"/>
-      <c r="N57" s="268"/>
-      <c r="O57" s="268"/>
-      <c r="P57" s="268"/>
-      <c r="Q57" s="268"/>
-      <c r="R57" s="268"/>
-      <c r="S57" s="268"/>
-      <c r="T57" s="269"/>
+      <c r="I57" s="295"/>
+      <c r="J57" s="295"/>
+      <c r="K57" s="295"/>
+      <c r="L57" s="295"/>
+      <c r="M57" s="268"/>
+      <c r="N57" s="269"/>
+      <c r="O57" s="269"/>
+      <c r="P57" s="269"/>
+      <c r="Q57" s="269"/>
+      <c r="R57" s="269"/>
+      <c r="S57" s="269"/>
+      <c r="T57" s="270"/>
       <c r="U57" s="133"/>
       <c r="V57" s="132"/>
       <c r="W57" s="132"/>
@@ -10542,18 +10292,18 @@
       <c r="F58" s="139"/>
       <c r="G58" s="139"/>
       <c r="H58" s="140"/>
-      <c r="I58" s="296"/>
-      <c r="J58" s="296"/>
-      <c r="K58" s="296"/>
-      <c r="L58" s="296"/>
-      <c r="M58" s="267"/>
-      <c r="N58" s="268"/>
-      <c r="O58" s="268"/>
-      <c r="P58" s="268"/>
-      <c r="Q58" s="268"/>
-      <c r="R58" s="268"/>
-      <c r="S58" s="268"/>
-      <c r="T58" s="269"/>
+      <c r="I58" s="295"/>
+      <c r="J58" s="295"/>
+      <c r="K58" s="295"/>
+      <c r="L58" s="295"/>
+      <c r="M58" s="268"/>
+      <c r="N58" s="269"/>
+      <c r="O58" s="269"/>
+      <c r="P58" s="269"/>
+      <c r="Q58" s="269"/>
+      <c r="R58" s="269"/>
+      <c r="S58" s="269"/>
+      <c r="T58" s="270"/>
       <c r="U58" s="133"/>
       <c r="V58" s="132"/>
       <c r="W58" s="132"/>
@@ -10576,18 +10326,18 @@
       <c r="F59" s="141"/>
       <c r="G59" s="141"/>
       <c r="H59" s="142"/>
-      <c r="I59" s="296"/>
-      <c r="J59" s="296"/>
-      <c r="K59" s="296"/>
-      <c r="L59" s="296"/>
-      <c r="M59" s="270"/>
-      <c r="N59" s="271"/>
-      <c r="O59" s="271"/>
-      <c r="P59" s="271"/>
-      <c r="Q59" s="271"/>
-      <c r="R59" s="271"/>
-      <c r="S59" s="271"/>
-      <c r="T59" s="272"/>
+      <c r="I59" s="295"/>
+      <c r="J59" s="295"/>
+      <c r="K59" s="295"/>
+      <c r="L59" s="295"/>
+      <c r="M59" s="271"/>
+      <c r="N59" s="272"/>
+      <c r="O59" s="272"/>
+      <c r="P59" s="272"/>
+      <c r="Q59" s="272"/>
+      <c r="R59" s="272"/>
+      <c r="S59" s="272"/>
+      <c r="T59" s="273"/>
       <c r="U59" s="133"/>
       <c r="V59" s="132"/>
       <c r="W59" s="132"/>
@@ -10673,28 +10423,28 @@
       <c r="C62" s="147"/>
       <c r="D62" s="147"/>
       <c r="E62" s="148"/>
-      <c r="F62" s="259" t="s">
+      <c r="F62" s="260" t="s">
         <v>241</v>
       </c>
-      <c r="G62" s="259"/>
-      <c r="H62" s="259"/>
-      <c r="I62" s="259"/>
-      <c r="J62" s="259"/>
-      <c r="K62" s="297"/>
-      <c r="L62" s="297"/>
-      <c r="M62" s="297"/>
-      <c r="N62" s="297"/>
-      <c r="O62" s="297"/>
-      <c r="P62" s="258"/>
-      <c r="Q62" s="258"/>
-      <c r="R62" s="258"/>
-      <c r="S62" s="258"/>
-      <c r="T62" s="258"/>
-      <c r="U62" s="258"/>
-      <c r="V62" s="258"/>
-      <c r="W62" s="258"/>
-      <c r="X62" s="258"/>
-      <c r="Y62" s="258"/>
+      <c r="G62" s="260"/>
+      <c r="H62" s="260"/>
+      <c r="I62" s="260"/>
+      <c r="J62" s="260"/>
+      <c r="K62" s="296"/>
+      <c r="L62" s="296"/>
+      <c r="M62" s="296"/>
+      <c r="N62" s="296"/>
+      <c r="O62" s="296"/>
+      <c r="P62" s="259"/>
+      <c r="Q62" s="259"/>
+      <c r="R62" s="259"/>
+      <c r="S62" s="259"/>
+      <c r="T62" s="259"/>
+      <c r="U62" s="259"/>
+      <c r="V62" s="259"/>
+      <c r="W62" s="259"/>
+      <c r="X62" s="259"/>
+      <c r="Y62" s="259"/>
       <c r="Z62" s="56"/>
       <c r="AA62" s="56"/>
       <c r="AB62" s="56"/>
@@ -10707,37 +10457,37 @@
         <v>26</v>
       </c>
       <c r="C63" s="150"/>
-      <c r="D63" s="294" t="s">
+      <c r="D63" s="293" t="s">
         <v>27</v>
       </c>
-      <c r="E63" s="295"/>
-      <c r="F63" s="259" t="s">
+      <c r="E63" s="294"/>
+      <c r="F63" s="260" t="s">
         <v>242</v>
       </c>
-      <c r="G63" s="259"/>
-      <c r="H63" s="259"/>
-      <c r="I63" s="259"/>
-      <c r="J63" s="259"/>
-      <c r="K63" s="297"/>
-      <c r="L63" s="297"/>
-      <c r="M63" s="297"/>
-      <c r="N63" s="297"/>
-      <c r="O63" s="297"/>
-      <c r="P63" s="297"/>
-      <c r="Q63" s="297"/>
-      <c r="R63" s="297"/>
-      <c r="S63" s="297"/>
-      <c r="T63" s="297"/>
-      <c r="U63" s="297"/>
-      <c r="V63" s="297"/>
-      <c r="W63" s="297"/>
-      <c r="X63" s="297"/>
-      <c r="Y63" s="297"/>
-      <c r="Z63" s="306"/>
-      <c r="AA63" s="306"/>
-      <c r="AB63" s="306"/>
-      <c r="AC63" s="306"/>
-      <c r="AD63" s="306"/>
+      <c r="G63" s="260"/>
+      <c r="H63" s="260"/>
+      <c r="I63" s="260"/>
+      <c r="J63" s="260"/>
+      <c r="K63" s="296"/>
+      <c r="L63" s="296"/>
+      <c r="M63" s="296"/>
+      <c r="N63" s="296"/>
+      <c r="O63" s="296"/>
+      <c r="P63" s="296"/>
+      <c r="Q63" s="296"/>
+      <c r="R63" s="296"/>
+      <c r="S63" s="296"/>
+      <c r="T63" s="296"/>
+      <c r="U63" s="296"/>
+      <c r="V63" s="296"/>
+      <c r="W63" s="296"/>
+      <c r="X63" s="296"/>
+      <c r="Y63" s="296"/>
+      <c r="Z63" s="305"/>
+      <c r="AA63" s="305"/>
+      <c r="AB63" s="305"/>
+      <c r="AC63" s="305"/>
+      <c r="AD63" s="305"/>
     </row>
     <row r="64" spans="1:30" ht="17.25" customHeight="1">
       <c r="A64" s="65"/>
@@ -10747,33 +10497,33 @@
       <c r="C64" s="147"/>
       <c r="D64" s="147"/>
       <c r="E64" s="148"/>
-      <c r="F64" s="259" t="s">
+      <c r="F64" s="260" t="s">
         <v>243</v>
       </c>
-      <c r="G64" s="259"/>
-      <c r="H64" s="259"/>
-      <c r="I64" s="259"/>
-      <c r="J64" s="259"/>
-      <c r="K64" s="297"/>
-      <c r="L64" s="297"/>
-      <c r="M64" s="297"/>
-      <c r="N64" s="297"/>
-      <c r="O64" s="297"/>
-      <c r="P64" s="297"/>
-      <c r="Q64" s="297"/>
-      <c r="R64" s="297"/>
-      <c r="S64" s="297"/>
-      <c r="T64" s="297"/>
-      <c r="U64" s="297"/>
-      <c r="V64" s="297"/>
-      <c r="W64" s="297"/>
-      <c r="X64" s="297"/>
-      <c r="Y64" s="297"/>
-      <c r="Z64" s="306"/>
-      <c r="AA64" s="306"/>
-      <c r="AB64" s="306"/>
-      <c r="AC64" s="306"/>
-      <c r="AD64" s="306"/>
+      <c r="G64" s="260"/>
+      <c r="H64" s="260"/>
+      <c r="I64" s="260"/>
+      <c r="J64" s="260"/>
+      <c r="K64" s="296"/>
+      <c r="L64" s="296"/>
+      <c r="M64" s="296"/>
+      <c r="N64" s="296"/>
+      <c r="O64" s="296"/>
+      <c r="P64" s="296"/>
+      <c r="Q64" s="296"/>
+      <c r="R64" s="296"/>
+      <c r="S64" s="296"/>
+      <c r="T64" s="296"/>
+      <c r="U64" s="296"/>
+      <c r="V64" s="296"/>
+      <c r="W64" s="296"/>
+      <c r="X64" s="296"/>
+      <c r="Y64" s="296"/>
+      <c r="Z64" s="305"/>
+      <c r="AA64" s="305"/>
+      <c r="AB64" s="305"/>
+      <c r="AC64" s="305"/>
+      <c r="AD64" s="305"/>
     </row>
     <row r="65" spans="1:30" ht="17.25" customHeight="1">
       <c r="A65" s="65"/>
@@ -10783,33 +10533,33 @@
       <c r="C65" s="147"/>
       <c r="D65" s="147"/>
       <c r="E65" s="148"/>
-      <c r="F65" s="259" t="s">
+      <c r="F65" s="260" t="s">
         <v>244</v>
       </c>
-      <c r="G65" s="259"/>
-      <c r="H65" s="259"/>
-      <c r="I65" s="259"/>
-      <c r="J65" s="259"/>
-      <c r="K65" s="308"/>
-      <c r="L65" s="308"/>
-      <c r="M65" s="308"/>
-      <c r="N65" s="308"/>
-      <c r="O65" s="308"/>
-      <c r="P65" s="308"/>
-      <c r="Q65" s="308"/>
-      <c r="R65" s="308"/>
-      <c r="S65" s="308"/>
-      <c r="T65" s="308"/>
-      <c r="U65" s="308"/>
-      <c r="V65" s="308"/>
-      <c r="W65" s="308"/>
-      <c r="X65" s="308"/>
-      <c r="Y65" s="308"/>
-      <c r="Z65" s="306"/>
-      <c r="AA65" s="306"/>
-      <c r="AB65" s="306"/>
-      <c r="AC65" s="306"/>
-      <c r="AD65" s="306"/>
+      <c r="G65" s="260"/>
+      <c r="H65" s="260"/>
+      <c r="I65" s="260"/>
+      <c r="J65" s="260"/>
+      <c r="K65" s="307"/>
+      <c r="L65" s="307"/>
+      <c r="M65" s="307"/>
+      <c r="N65" s="307"/>
+      <c r="O65" s="307"/>
+      <c r="P65" s="307"/>
+      <c r="Q65" s="307"/>
+      <c r="R65" s="307"/>
+      <c r="S65" s="307"/>
+      <c r="T65" s="307"/>
+      <c r="U65" s="307"/>
+      <c r="V65" s="307"/>
+      <c r="W65" s="307"/>
+      <c r="X65" s="307"/>
+      <c r="Y65" s="307"/>
+      <c r="Z65" s="305"/>
+      <c r="AA65" s="305"/>
+      <c r="AB65" s="305"/>
+      <c r="AC65" s="305"/>
+      <c r="AD65" s="305"/>
     </row>
     <row r="66" spans="1:30" ht="17.25" customHeight="1">
       <c r="A66" s="65"/>
@@ -10819,69 +10569,69 @@
       <c r="C66" s="147"/>
       <c r="D66" s="147"/>
       <c r="E66" s="148"/>
-      <c r="F66" s="259" t="s">
+      <c r="F66" s="260" t="s">
         <v>245</v>
       </c>
-      <c r="G66" s="259"/>
-      <c r="H66" s="259"/>
-      <c r="I66" s="259"/>
-      <c r="J66" s="259"/>
-      <c r="K66" s="308"/>
-      <c r="L66" s="308"/>
-      <c r="M66" s="308"/>
-      <c r="N66" s="308"/>
-      <c r="O66" s="308"/>
-      <c r="P66" s="308"/>
-      <c r="Q66" s="308"/>
-      <c r="R66" s="308"/>
-      <c r="S66" s="308"/>
-      <c r="T66" s="308"/>
-      <c r="U66" s="308"/>
-      <c r="V66" s="308"/>
-      <c r="W66" s="308"/>
-      <c r="X66" s="308"/>
-      <c r="Y66" s="308"/>
-      <c r="Z66" s="307"/>
-      <c r="AA66" s="307"/>
-      <c r="AB66" s="307"/>
-      <c r="AC66" s="307"/>
-      <c r="AD66" s="307"/>
+      <c r="G66" s="260"/>
+      <c r="H66" s="260"/>
+      <c r="I66" s="260"/>
+      <c r="J66" s="260"/>
+      <c r="K66" s="307"/>
+      <c r="L66" s="307"/>
+      <c r="M66" s="307"/>
+      <c r="N66" s="307"/>
+      <c r="O66" s="307"/>
+      <c r="P66" s="307"/>
+      <c r="Q66" s="307"/>
+      <c r="R66" s="307"/>
+      <c r="S66" s="307"/>
+      <c r="T66" s="307"/>
+      <c r="U66" s="307"/>
+      <c r="V66" s="307"/>
+      <c r="W66" s="307"/>
+      <c r="X66" s="307"/>
+      <c r="Y66" s="307"/>
+      <c r="Z66" s="306"/>
+      <c r="AA66" s="306"/>
+      <c r="AB66" s="306"/>
+      <c r="AC66" s="306"/>
+      <c r="AD66" s="306"/>
     </row>
     <row r="67" spans="1:30" ht="17.25" customHeight="1">
       <c r="A67" s="65"/>
-      <c r="B67" s="293" t="s">
+      <c r="B67" s="292" t="s">
         <v>49</v>
       </c>
-      <c r="C67" s="294"/>
-      <c r="D67" s="294"/>
-      <c r="E67" s="295"/>
-      <c r="F67" s="259" t="s">
+      <c r="C67" s="293"/>
+      <c r="D67" s="293"/>
+      <c r="E67" s="294"/>
+      <c r="F67" s="260" t="s">
         <v>246</v>
       </c>
-      <c r="G67" s="259"/>
-      <c r="H67" s="259"/>
-      <c r="I67" s="259"/>
-      <c r="J67" s="259"/>
-      <c r="K67" s="308"/>
-      <c r="L67" s="308"/>
-      <c r="M67" s="308"/>
-      <c r="N67" s="308"/>
-      <c r="O67" s="308"/>
-      <c r="P67" s="308"/>
-      <c r="Q67" s="308"/>
-      <c r="R67" s="308"/>
-      <c r="S67" s="308"/>
-      <c r="T67" s="308"/>
-      <c r="U67" s="308"/>
-      <c r="V67" s="308"/>
-      <c r="W67" s="308"/>
-      <c r="X67" s="308"/>
-      <c r="Y67" s="308"/>
-      <c r="Z67" s="307"/>
-      <c r="AA67" s="307"/>
-      <c r="AB67" s="307"/>
-      <c r="AC67" s="307"/>
-      <c r="AD67" s="307"/>
+      <c r="G67" s="260"/>
+      <c r="H67" s="260"/>
+      <c r="I67" s="260"/>
+      <c r="J67" s="260"/>
+      <c r="K67" s="307"/>
+      <c r="L67" s="307"/>
+      <c r="M67" s="307"/>
+      <c r="N67" s="307"/>
+      <c r="O67" s="307"/>
+      <c r="P67" s="307"/>
+      <c r="Q67" s="307"/>
+      <c r="R67" s="307"/>
+      <c r="S67" s="307"/>
+      <c r="T67" s="307"/>
+      <c r="U67" s="307"/>
+      <c r="V67" s="307"/>
+      <c r="W67" s="307"/>
+      <c r="X67" s="307"/>
+      <c r="Y67" s="307"/>
+      <c r="Z67" s="306"/>
+      <c r="AA67" s="306"/>
+      <c r="AB67" s="306"/>
+      <c r="AC67" s="306"/>
+      <c r="AD67" s="306"/>
     </row>
     <row r="68" spans="1:30" ht="17.25" customHeight="1">
       <c r="A68" s="65"/>
@@ -10891,28 +10641,28 @@
       <c r="C68" s="147"/>
       <c r="D68" s="147"/>
       <c r="E68" s="148"/>
-      <c r="F68" s="259" t="s">
+      <c r="F68" s="260" t="s">
         <v>247</v>
       </c>
-      <c r="G68" s="259"/>
-      <c r="H68" s="259"/>
-      <c r="I68" s="259"/>
-      <c r="J68" s="259"/>
-      <c r="K68" s="292"/>
-      <c r="L68" s="292"/>
-      <c r="M68" s="292"/>
-      <c r="N68" s="292"/>
-      <c r="O68" s="292"/>
-      <c r="P68" s="292"/>
-      <c r="Q68" s="292"/>
-      <c r="R68" s="292"/>
-      <c r="S68" s="292"/>
-      <c r="T68" s="292"/>
-      <c r="U68" s="292"/>
-      <c r="V68" s="292"/>
-      <c r="W68" s="292"/>
-      <c r="X68" s="292"/>
-      <c r="Y68" s="292"/>
+      <c r="G68" s="260"/>
+      <c r="H68" s="260"/>
+      <c r="I68" s="260"/>
+      <c r="J68" s="260"/>
+      <c r="K68" s="291"/>
+      <c r="L68" s="291"/>
+      <c r="M68" s="291"/>
+      <c r="N68" s="291"/>
+      <c r="O68" s="291"/>
+      <c r="P68" s="291"/>
+      <c r="Q68" s="291"/>
+      <c r="R68" s="291"/>
+      <c r="S68" s="291"/>
+      <c r="T68" s="291"/>
+      <c r="U68" s="291"/>
+      <c r="V68" s="291"/>
+      <c r="W68" s="291"/>
+      <c r="X68" s="291"/>
+      <c r="Y68" s="291"/>
       <c r="Z68" s="151"/>
       <c r="AA68" s="152"/>
       <c r="AB68" s="151"/>
@@ -10927,33 +10677,33 @@
       <c r="C69" s="147"/>
       <c r="D69" s="147"/>
       <c r="E69" s="148"/>
-      <c r="F69" s="259" t="s">
+      <c r="F69" s="260" t="s">
         <v>248</v>
       </c>
-      <c r="G69" s="259"/>
-      <c r="H69" s="259"/>
-      <c r="I69" s="259"/>
-      <c r="J69" s="259"/>
-      <c r="K69" s="309"/>
-      <c r="L69" s="309"/>
-      <c r="M69" s="309"/>
-      <c r="N69" s="309"/>
-      <c r="O69" s="309"/>
-      <c r="P69" s="309"/>
-      <c r="Q69" s="309"/>
-      <c r="R69" s="309"/>
-      <c r="S69" s="309"/>
-      <c r="T69" s="309"/>
-      <c r="U69" s="309"/>
-      <c r="V69" s="309"/>
-      <c r="W69" s="309"/>
-      <c r="X69" s="309"/>
-      <c r="Y69" s="309"/>
-      <c r="Z69" s="306"/>
-      <c r="AA69" s="306"/>
-      <c r="AB69" s="306"/>
-      <c r="AC69" s="306"/>
-      <c r="AD69" s="306"/>
+      <c r="G69" s="260"/>
+      <c r="H69" s="260"/>
+      <c r="I69" s="260"/>
+      <c r="J69" s="260"/>
+      <c r="K69" s="308"/>
+      <c r="L69" s="308"/>
+      <c r="M69" s="308"/>
+      <c r="N69" s="308"/>
+      <c r="O69" s="308"/>
+      <c r="P69" s="308"/>
+      <c r="Q69" s="308"/>
+      <c r="R69" s="308"/>
+      <c r="S69" s="308"/>
+      <c r="T69" s="308"/>
+      <c r="U69" s="308"/>
+      <c r="V69" s="308"/>
+      <c r="W69" s="308"/>
+      <c r="X69" s="308"/>
+      <c r="Y69" s="308"/>
+      <c r="Z69" s="305"/>
+      <c r="AA69" s="305"/>
+      <c r="AB69" s="305"/>
+      <c r="AC69" s="305"/>
+      <c r="AD69" s="305"/>
     </row>
     <row r="70" spans="1:30" ht="13.5" customHeight="1">
       <c r="A70" s="65"/>
@@ -10963,27 +10713,27 @@
       <c r="C70" s="147"/>
       <c r="D70" s="147"/>
       <c r="E70" s="148"/>
-      <c r="F70" s="313" t="s">
+      <c r="F70" s="312" t="s">
         <v>249</v>
       </c>
-      <c r="G70" s="314"/>
-      <c r="H70" s="314"/>
-      <c r="I70" s="314"/>
-      <c r="J70" s="315"/>
+      <c r="G70" s="313"/>
+      <c r="H70" s="313"/>
+      <c r="I70" s="313"/>
+      <c r="J70" s="314"/>
       <c r="K70" s="110"/>
-      <c r="L70" s="297"/>
-      <c r="M70" s="297"/>
-      <c r="N70" s="297"/>
+      <c r="L70" s="296"/>
+      <c r="M70" s="296"/>
+      <c r="N70" s="296"/>
       <c r="O70" s="110"/>
       <c r="P70" s="110"/>
-      <c r="Q70" s="297"/>
-      <c r="R70" s="297"/>
-      <c r="S70" s="297"/>
+      <c r="Q70" s="296"/>
+      <c r="R70" s="296"/>
+      <c r="S70" s="296"/>
       <c r="T70" s="110"/>
       <c r="U70" s="110"/>
-      <c r="V70" s="297"/>
-      <c r="W70" s="297"/>
-      <c r="X70" s="297"/>
+      <c r="V70" s="296"/>
+      <c r="W70" s="296"/>
+      <c r="X70" s="296"/>
       <c r="Y70" s="110"/>
       <c r="Z70" s="56"/>
       <c r="AA70" s="56"/>
@@ -11029,10 +10779,10 @@
       <c r="N72" s="156"/>
     </row>
     <row r="73" spans="1:30" ht="17.25" customHeight="1">
-      <c r="J73" s="311"/>
-      <c r="K73" s="312"/>
-      <c r="L73" s="312"/>
-      <c r="M73" s="312"/>
+      <c r="J73" s="310"/>
+      <c r="K73" s="311"/>
+      <c r="L73" s="311"/>
+      <c r="M73" s="311"/>
       <c r="W73" s="157"/>
     </row>
     <row r="75" spans="1:30" ht="17.25" customHeight="1">
@@ -11090,6 +10840,7 @@
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E18:F18"/>
+    <mergeCell ref="P10:W10"/>
     <mergeCell ref="AF20:AF21"/>
     <mergeCell ref="AJ33:AL33"/>
     <mergeCell ref="AM33:AN33"/>
@@ -11250,7 +11001,6 @@
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="M15:N15"/>
     <mergeCell ref="H26:I26"/>
-    <mergeCell ref="P10:W10"/>
     <mergeCell ref="P11:V11"/>
     <mergeCell ref="X10:AA10"/>
     <mergeCell ref="I52:L52"/>
@@ -37698,21 +37448,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004D4CCBE22655944796F59B17B9006C15" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f481576c72d824a80c867b56d5274a41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b7c6cbfa-29cf-4ada-90bf-db8e550dae8d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3bc755a260c778b5f630b987d93a78f8" ns2:_="">
     <xsd:import namespace="b7c6cbfa-29cf-4ada-90bf-db8e550dae8d"/>
@@ -37890,7 +37625,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82807CA0-8C25-4FF6-8C67-D0A8F7400434}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b7c6cbfa-29cf-4ada-90bf-db8e550dae8d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECA946AD-4EA3-4FCA-B864-262800288FDF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -37906,28 +37674,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5458833A-D997-4113-BB83-F938CBB9D86E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82807CA0-8C25-4FF6-8C67-D0A8F7400434}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b7c6cbfa-29cf-4ada-90bf-db8e550dae8d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>